<commit_message>
Backend Facets Queries Answers
</commit_message>
<xml_diff>
--- a/Facets_Backend_CaseStudy Queries.xlsx
+++ b/Facets_Backend_CaseStudy Queries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2355482\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA430F43-C56E-4728-9596-ADD734746D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B1D3AF-58B8-425E-BD9C-CBE648C0C18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DF85CDAB-7E31-457A-ACB5-C0BF459524E0}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{DF85CDAB-7E31-457A-ACB5-C0BF459524E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Queries-Case StudyTemplate" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
   <si>
     <t>Question</t>
   </si>
@@ -251,6 +251,52 @@
 AND NWPR.NWPR_EFF_DT &lt; GETDATE() AND NWPR.NWPR_TERM_DT  &gt; GETDATE()
 AND NWST.NWST_EFF_DT &lt;GETDATE() AND NWST.NWST_TERM_DT &gt;GETDATE()
 AND CSPI.CSPI_EFF_DT &lt;GETDATE() AND CSPI.CSPI_TERM_DT&gt;GETDATE();</t>
+  </si>
+  <si>
+    <t>SELECT CL.CLCL_ID, CL.CLCL_CUR_STS 
+FROM CMC_CLCL_CLAIM CL,  CMC_SBSB_SUBSC SB 
+WHERE CL.SBSB_CK = SB.SBSB_CK  
+AND CL.CLCL_CUR_STS = '11' AND SB.SBSB_ID = '070700003' AND SB.SBSB_ORIG_EFF_DT&lt;=GETDATE() AND SB.SBSB_MCTR_STS = 'ACTI';</t>
+  </si>
+  <si>
+    <t>SELECT CL.CLCL_ID, CL.CLCL_CL_TYPE, CL.CLCL_CL_SUB_TYPE
+FROM CMC_CLCL_CLAIM CL, CMC_SBSB_SUBSC SB
+WHERE CL.SBSB_CK = SB.SBSB_CK AND (CL.CLCL_CUR_STS = 11 OR CL.CLCL_CUR_STS = 15) 
+AND SB.SBSB_ID = '070700003' AND SB.SBSB_ORIG_EFF_DT&lt;=GETDATE()  AND  SB.SBSB_MCTR_STS='ACTI';</t>
+  </si>
+  <si>
+    <t>SELECT PR.PRPR_NAME, CD.IPCD_ID, CD.IDCD_ID 
+FROM CMC_CLCL_CLAIM CL, CMC_CDML_CL_LINE CD, CMC_PRPR_PROV PR
+WHERE CL.CLCL_ID = CD.CLCL_ID AND CD.PRPR_ID = PR.PRPR_ID AND CL.PRPR_ID = PR.PRPR_ID
+AND CL.CLCL_ID = '072180000100';</t>
+  </si>
+  <si>
+    <t>SELECT pypy.PYPY_PAYOR_NAME, pyba.PYBA_BANK_NAME
+FROM CMC_CLCK_CLM_CHECK clck, CMC_LOBD_LINE_BUS lobd, CMC_PYPY_PAYOR pypy, CMC_PYBA_BANK_ACCT pyba
+WHERE clck.LOBD_ID = lobd.LOBD_ID
+AND pypy.PYBA_ID = pyba.PYBA_ID
+AND lobd.PYPY_ID = pypy.PYPY_ID 
+AND clck.CLCL_ID = '072180000100' 
+AND GETDATE() BETWEEN pypy.PYPY_EFF_DT AND pypy.PYPY_TERM_DT</t>
+  </si>
+  <si>
+    <t>SELECT CLCK.CKPY_REF_ID FROM CMC_CDML_CL_LINE CDML,CMC_CLCK_CLM_CHECK CLCK
+WHERE CDML.CLCL_ID=CLCK.CLCL_ID
+AND CDML.CLCL_ID='072180000100';</t>
+  </si>
+  <si>
+    <t>SELECT CLOV_AMT FROM CMC_CLOV_OVERPAY WHERE CLCL_ID = '072200000401';</t>
+  </si>
+  <si>
+    <t>SELECT ACPR.ACPR_RECOV_AMT, ACPR.ACPR_REF_ID
+FROM CMC_ACPR_PYMT_RED ACPR, CMC_LOBD_LINE_BUS LOBD, CMC_CLCK_CLM_CHECK CLCK
+WHERE ACPR.LOBD_ID = LOBD.LOBD_ID AND LOBD.LOBD_ID = CLCK.LOBD_ID AND CLCK.CLCL_ID = '072200000401'</t>
+  </si>
+  <si>
+    <t>SELECT CKPY.CKPY_REF_ID, ACPR.ACPR_RECOV_AMT
+FROM CMC_CLCK_CLM_CHECK CLCK, CMC_LOBD_LINE_BUS LOBD, CMC_CKPY_PAYEE_SUM CKPY, CMC_ACRH_RED_HIST ACRH, CMC_ACPR_PYMT_RED ACPR
+WHERE CLCK.LOBD_ID = LOBD.LOBD_ID AND LOBD.LOBD_ID = CKPY.LOBD_ID AND CKPY.CKPY_REF_ID = ACRH.CKPY_REF_ID AND ACRH.ACPR_REF_ID = ACPR.ACPR_REF_ID
+AND CLCK.CLCL_ID = '072200000401'</t>
   </si>
 </sst>
 </file>
@@ -677,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCB8316-C7F4-42B9-80FF-38C0E1A43232}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1098,62 +1144,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="6"/>
+      <c r="C30" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="D30" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="6"/>
+      <c r="C31" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="D31" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>3</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="6"/>
+      <c r="C32" s="12" t="s">
+        <v>45</v>
+      </c>
       <c r="D32" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="91.5" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>4</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="6"/>
+      <c r="C33" s="12" t="s">
+        <v>46</v>
+      </c>
       <c r="D33" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>5</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="6"/>
+      <c r="C34" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="D34" s="2">
         <v>1</v>
       </c>
@@ -1165,31 +1221,37 @@
       <c r="B35" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="6"/>
+      <c r="C35" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="D35" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>7</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="6"/>
+      <c r="C36" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="D36" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>8</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="6"/>
+      <c r="C37" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="D37" s="2">
         <v>1</v>
       </c>

</xml_diff>